<commit_message>
Excel com tempo de duração dos testes
</commit_message>
<xml_diff>
--- a/FuzzyAI/report.xlsx
+++ b/FuzzyAI/report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Escola\3º ano\2º semestre\Projeto_Final\FuzzyAI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Escola\3º ano\2º semestre\Projeto_Final\llmSecurity\FuzzyAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B665044A-2A50-414C-B0D7-5A72225499CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F6E825-70CF-465F-B3AB-A29BE6FACD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>prompt</t>
   </si>
@@ -43,13 +43,20 @@
   </si>
   <si>
     <t>modelo a ser atacado</t>
+  </si>
+  <si>
+    <t>runtime</t>
+  </si>
+  <si>
+    <t>Duração do ataque, em segundos: 
+(Atenção! A duração do ataque vai ser sempre superior à soma do 'runtime' de cada prompt)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,8 +64,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -68,6 +83,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -84,7 +105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -93,6 +114,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,93 +397,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="78.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.109375" customWidth="1"/>
     <col min="4" max="4" width="56.5546875" customWidth="1"/>
     <col min="5" max="5" width="72.77734375" customWidth="1"/>
     <col min="6" max="6" width="9.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="F2"/>
-    </row>
-    <row r="3" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="B3"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4"/>
       <c r="B4"/>
       <c r="F4"/>
     </row>
-    <row r="5" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5"/>
       <c r="B5"/>
       <c r="F5"/>
     </row>
-    <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6"/>
       <c r="B6"/>
       <c r="F6"/>
     </row>
-    <row r="7" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7"/>
       <c r="B7"/>
       <c r="F7"/>
     </row>
-    <row r="8" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8"/>
       <c r="B8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9"/>
       <c r="B9"/>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10"/>
       <c r="B10"/>
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="B11"/>
       <c r="F11"/>
     </row>
-    <row r="13" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="F12"/>
+    </row>
+    <row r="14" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
argumento 'language' traducao de ataques
</commit_message>
<xml_diff>
--- a/FuzzyAI/report.xlsx
+++ b/FuzzyAI/report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Escola\3º ano\2º semestre\Projeto_Final\llmSecurity\FuzzyAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F6E825-70CF-465F-B3AB-A29BE6FACD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88BA5AD-05EE-4EAB-8467-004A25510FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
   </si>
   <si>
     <t>Duração do ataque, em segundos: 
-(Atenção! A duração do ataque vai ser sempre superior à soma do 'runtime' de cada prompt)</t>
+(Atenção! A duração total do ataque pode ser superior à soma do 'runtime' de cada prompt)</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>